<commit_message>
Additional translation, standardization and missing data to management files.
</commit_message>
<xml_diff>
--- a/data/management/Management_information_DKI_2016.xlsx
+++ b/data/management/Management_information_DKI_2016.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillrose/Library/Mobile Documents/com~apple~CloudDocs/iCloud Daten/Arbeit/R-Projects/Git_Repositories/BRIWECS_Data_Publication_2/data/management/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA01D26-9CA9-4B4C-A52C-7ACA54B55955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="450" windowWidth="19440" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="29500" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t xml:space="preserve">Correspondence </t>
   </si>
@@ -229,9 +235,6 @@
     <t>Hohenschulen, Achterwehr</t>
   </si>
   <si>
-    <t>KAS</t>
-  </si>
-  <si>
     <t>1.0l CCC + 0.2l Calma</t>
   </si>
   <si>
@@ -301,12 +304,6 @@
     <t>Hohenschulen (eigen)</t>
   </si>
   <si>
-    <t>others</t>
-  </si>
-  <si>
-    <t>5 kg Bittersalz + 0.7l Mangan + 0.3l Kupfer</t>
-  </si>
-  <si>
     <t>0.4l</t>
   </si>
   <si>
@@ -340,12 +337,6 @@
     <t>0.2l Moddus + 0.2l Profi Etephon</t>
   </si>
   <si>
-    <t>Alzon 40 + 5 S</t>
-  </si>
-  <si>
-    <t>Bittersalz</t>
-  </si>
-  <si>
     <t>Amount kg/ha</t>
   </si>
   <si>
@@ -353,12 +344,18 @@
   </si>
   <si>
     <t>Parabraunerde/Pseudogley</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>UAN (inhibited)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,10 +556,10 @@
     <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20 % - Akzent3" xfId="3" builtinId="38"/>
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
-    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,14 +567,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -615,7 +615,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -687,7 +687,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -860,32 +860,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" customWidth="1"/>
+    <col min="11" max="11" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -893,7 +894,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -901,7 +902,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -909,7 +910,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -917,7 +918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -925,15 +926,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -941,163 +942,163 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="B18" s="14">
         <v>42282</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1106,7 +1107,7 @@
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1115,7 +1116,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
@@ -1124,7 +1125,7 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>41518</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1144,91 +1145,91 @@
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="14">
         <v>41518</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="14">
         <v>41518</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="14">
         <v>42436</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" s="14">
         <v>42436</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="14">
         <v>42436</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="14">
         <v>42436</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>65</v>
       </c>
@@ -1243,7 +1244,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>53</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>6</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>7</v>
@@ -1266,7 +1267,7 @@
         <v>6</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>7</v>
@@ -1278,7 +1279,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>50</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>12</v>
@@ -1301,29 +1302,31 @@
         <v>42300</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>56</v>
       </c>
       <c r="K47" s="8"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="11"/>
+      <c r="C48" s="11">
+        <v>42473</v>
+      </c>
       <c r="D48" s="6">
         <v>80</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>13</v>
@@ -1332,7 +1335,7 @@
         <v>42492</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="8" t="s">
@@ -1340,19 +1343,21 @@
       </c>
       <c r="K48" s="8"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="11"/>
+      <c r="C49" s="11">
+        <v>42474</v>
+      </c>
       <c r="D49" s="6">
         <v>60</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>14</v>
@@ -1361,35 +1366,29 @@
         <v>42530</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J49" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="11">
-        <v>42453</v>
-      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="13" t="s">
-        <v>96</v>
-      </c>
+      <c r="E50" s="13"/>
       <c r="F50" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -1398,20 +1397,14 @@
       </c>
       <c r="K50" s="8"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>66</v>
       </c>
       <c r="B51" s="13"/>
-      <c r="C51" s="11">
-        <v>42492</v>
-      </c>
-      <c r="D51" s="13">
-        <v>3</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>109</v>
-      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="7" t="s">
         <v>16</v>
       </c>
@@ -1419,7 +1412,7 @@
         <v>42492</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="8" t="s">
@@ -1427,20 +1420,14 @@
       </c>
       <c r="K51" s="8"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>66</v>
       </c>
       <c r="B52" s="6"/>
-      <c r="C52" s="11">
-        <v>42509</v>
-      </c>
-      <c r="D52" s="13">
-        <v>3</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>109</v>
-      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
       <c r="F52" s="7" t="s">
         <v>17</v>
       </c>
@@ -1448,7 +1435,7 @@
         <v>42509</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="8" t="s">
@@ -1456,7 +1443,7 @@
       </c>
       <c r="K52" s="8"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1471,15 +1458,15 @@
         <v>42530</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -1494,13 +1481,13 @@
         <v>42492</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -1515,7 +1502,7 @@
         <v>42509</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I55" s="7"/>
       <c r="J55" s="8"/>

</xml_diff>